<commit_message>
feat: Delete app files from this repo
</commit_message>
<xml_diff>
--- a/example_file.xlsx
+++ b/example_file.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11003"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/icpe/phd/LMS-zscore-calculator/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bkh810/LMS-zscore-calculator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{280B6632-DFD2-E44A-BC8E-8B4D8B77E9F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11D4265E-8F77-AC42-BE65-5D402EA88536}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="17180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -433,12 +433,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AD8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="V8" sqref="V8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="5" max="5" width="18.5" customWidth="1"/>
+    <col min="6" max="6" width="27.6640625" customWidth="1"/>
+    <col min="7" max="7" width="25.1640625" customWidth="1"/>
+    <col min="8" max="8" width="20.5" customWidth="1"/>
     <col min="26" max="26" width="17.83203125" customWidth="1"/>
     <col min="27" max="27" width="16" customWidth="1"/>
     <col min="30" max="30" width="22.33203125" customWidth="1"/>
@@ -851,6 +855,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 

</xml_diff>